<commit_message>
modificaciones pequeñas a la dinamica
</commit_message>
<xml_diff>
--- a/Pristiamantis_acatallelus.xlsx
+++ b/Pristiamantis_acatallelus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnsov/Desktop/Proyectos de Investigación 2025/Ocupacion_Farallones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AD3D0E-744E-4642-9017-BC3F24B2430A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21A0B6D-3816-5B4C-A9DE-B179ACC9173F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="660" windowWidth="16580" windowHeight="18800" firstSheet="3" activeTab="10" xr2:uid="{0E724713-D368-CE48-B177-BB2AF005B536}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="16580" windowHeight="18800" firstSheet="3" activeTab="10" xr2:uid="{0E724713-D368-CE48-B177-BB2AF005B536}"/>
   </bookViews>
   <sheets>
     <sheet name="Notacion" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="40">
   <si>
     <t>T1</t>
   </si>
@@ -888,7 +888,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,7 +1144,9 @@
       <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="9">
         <v>1</v>
       </c>
@@ -1461,7 +1463,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1519,7 +1521,9 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1854,7 +1858,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>